<commit_message>
add  “-a .xlsx”  function to calculate the last -a rows of excel data
</commit_message>
<xml_diff>
--- a/Excelavg/bin/Debug/23空白.xlsx
+++ b/Excelavg/bin/Debug/23空白.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Project_VS\ExcelProj\Excelavg\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Project_VS\ExcelProj\Excel_avg\Excelavg\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56D8075-36F0-49E2-89E5-FF315E508667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF24457-DB44-4E35-A5F5-4F720B676D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="13700" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="790" yWindow="2470" windowWidth="9920" windowHeight="8330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>

</xml_diff>